<commit_message>
adding scripts for annotation pipeline”
</commit_message>
<xml_diff>
--- a/code/sctype_annotation/gs_listv4.xlsx
+++ b/code/sctype_annotation/gs_listv4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fallo\Documents\Internship_2023\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBA2F38-315A-4CC3-9CF2-6D0BFA91B90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E2BC96-BD9D-4003-8F41-A3696EBB6F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4046A3FF-AA47-4460-BC14-9146B2FEEA09}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Neuroepithelial cells</t>
   </si>
@@ -53,15 +53,6 @@
     <t>Neuroblasts</t>
   </si>
   <si>
-    <t>PVALB</t>
-  </si>
-  <si>
-    <t>SST</t>
-  </si>
-  <si>
-    <t>VIP</t>
-  </si>
-  <si>
     <t>OPCs</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>AGXT2L1,S100A1,SLC14A1L,GJA1,SLC1A2,SLC1A3,SLCO1C1,ALDH1L1</t>
   </si>
   <si>
-    <t>PECAM1,CD93,GBN,IL32,IGFPB7,FN1,CLDN5,VWF,TM4SF1,CD34,CDH5</t>
-  </si>
-  <si>
     <t>P2RY12,TMEM119,CX3CR1,ITGAM,TREM2</t>
   </si>
   <si>
@@ -158,12 +146,6 @@
     <t>Interneuron Precursors</t>
   </si>
   <si>
-    <t>ID2</t>
-  </si>
-  <si>
-    <t>NDNF</t>
-  </si>
-  <si>
     <t>PCP4,CNTN6,CTIP2,FOXP2,TLE4,CTGF,THEMIS,BCL11B,SOX5,LMO3</t>
   </si>
   <si>
@@ -179,18 +161,9 @@
     <t>GAD2,ASCL1,DLX2,BHLHE22,SOX4</t>
   </si>
   <si>
-    <t>NRG1,KIT,NRG1,CXCL14,CCK</t>
-  </si>
-  <si>
-    <t>NDNF,NMBR,CCK,RELN,LAMP5,SV2C</t>
-  </si>
-  <si>
     <t>NEUROD1,DCX,EOMES,TUBB3</t>
   </si>
   <si>
-    <t>LHX6, SOX6</t>
-  </si>
-  <si>
     <t>MGE INs</t>
   </si>
   <si>
@@ -221,24 +194,12 @@
     <t>SOX2,HOPX,PEA15,LGALS3BP,MOXD1,CLU,QKI</t>
   </si>
   <si>
-    <t>EMX2,SPARC,HELLS,DHFR,SOX2,VIM,ARHGAP11A,GLI3,HES1,EGR1</t>
-  </si>
-  <si>
     <t>DCX,INA,NEUROD6,EIF1B,MEIS2,FOXG1,MEF2C</t>
   </si>
   <si>
-    <t>LUZP2,PVALB,LHX6,SOX6,SLIT2,PCDH7,SULF1,WFDC2,SCUBE3</t>
-  </si>
-  <si>
-    <t>BCL11A,PDE1A,RALYL,SST,LHX6,SOX6,RELN,PCDH7</t>
-  </si>
-  <si>
     <t>STMN2,NEUROD6,LIMCH1,SYT4</t>
   </si>
   <si>
-    <t>VIP,CXCL14,CALB2,CRH,PCDH7,ABI3BP,ADAMTSL1</t>
-  </si>
-  <si>
     <t>NEUROD6</t>
   </si>
   <si>
@@ -252,6 +213,30 @@
   </si>
   <si>
     <t>Mixed</t>
+  </si>
+  <si>
+    <t>LHX6, SOX6,NKX2-1</t>
+  </si>
+  <si>
+    <t>SPARC,HELLS,DHFR,SOX2,VIM,ARHGAP11A,GLI3,HES1,EGR1,CRYAB</t>
+  </si>
+  <si>
+    <t>Glioblasts</t>
+  </si>
+  <si>
+    <t>TNC,BCAN</t>
+  </si>
+  <si>
+    <t>Mesenchmycal Cells</t>
+  </si>
+  <si>
+    <t>MSCs</t>
+  </si>
+  <si>
+    <t>PECAM1,CD93,GBN,IL32,IGFPB7,FN1,CLDN5,VWF,TM4SF1,CD34,CDH5,HBG,HBM</t>
+  </si>
+  <si>
+    <t>LUM,TBX1</t>
   </si>
 </sst>
 </file>
@@ -681,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E02F9-E482-4ABB-A20B-6BED7642B776}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -697,24 +682,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -724,432 +709,389 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7"/>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>57</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="1"/>
+      <c r="E34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>